<commit_message>
Assignment 13 completed 13%
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mukeshotwani/eclipse-workspace_newBatch_Sep_INeuron_2022_sep/HybridFramework/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sv70\Documents\GitHub\HybridFrameworkSep2022\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F119BD9-BF62-5546-8C53-1FF040D8A048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576F18A7-B04D-476A-A67E-8D5966AF1C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="36860" windowHeight="21600" xr2:uid="{5DD29F64-61B9-E248-8F90-E54ABE76EBE9}"/>
+    <workbookView xWindow="1425" yWindow="1545" windowWidth="21600" windowHeight="11385" xr2:uid="{5DD29F64-61B9-E248-8F90-E54ABE76EBE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -42,10 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>admin</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>Username</t>
   </si>
@@ -57,9 +54,6 @@
   </si>
   <si>
     <t>ineuron</t>
-  </si>
-  <si>
-    <t>admin@admin.com</t>
   </si>
 </sst>
 </file>
@@ -126,11 +120,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -439,7 +432,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -450,42 +443,42 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{B120ED97-6D07-1947-9B77-FE210F9A8959}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{B3157D8F-DECA-A345-BF6F-DF7442F8909F}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{ED1B86B6-CEE2-46AA-A3AA-42D2F64563A7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -497,7 +490,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -509,7 +502,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -521,7 +514,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -533,7 +526,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -545,7 +538,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -557,7 +550,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
excel data modified removed wrong credentials
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mukeshotwani/eclipse-workspace_newBatch_Sep_INeuron_2022_sep/HybridFramework/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l\git\HybridFrameworkSep2022\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F119BD9-BF62-5546-8C53-1FF040D8A048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="36860" windowHeight="21600" xr2:uid="{5DD29F64-61B9-E248-8F90-E54ABE76EBE9}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="36855" windowHeight="21600"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <sheet name="Sheet5" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet6" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,10 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>admin</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Username</t>
   </si>
@@ -58,14 +54,11 @@
   <si>
     <t>ineuron</t>
   </si>
-  <si>
-    <t>admin@admin.com</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -126,11 +119,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -446,118 +438,109 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02AB7364-1DB5-704A-8C2D-FD6EFD131388}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{B120ED97-6D07-1947-9B77-FE210F9A8959}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{B3157D8F-DECA-A345-BF6F-DF7442F8909F}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB18963-6236-664C-9EC0-1BF2B3E61C7F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E0A2A38-FCA8-0E44-986D-FD6C49996A2F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{694F4971-7C32-3B4A-8E6E-2A1A1E001E70}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C06EE55-DD61-3A4F-A6C9-133EF186A059}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC2849D3-09EB-E44A-86F4-59B8952AFE7C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E861318B-285F-1E48-9F82-9D5166D65256}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Push via SSH Key
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -1,47 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l\git\HybridFrameworkSep2022\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{5D95B635-6528-4424-B668-2393BD27BC00}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="36855" windowHeight="21600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14415" windowHeight="6015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="userdetails" sheetId="2" r:id="rId2"/>
+    <sheet name="checkuser" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet5" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet6" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:J16"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>Username</t>
   </si>
@@ -54,11 +40,29 @@
   <si>
     <t>ineuron</t>
   </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>pwdforUC</t>
+  </si>
+  <si>
+    <t>Chandan</t>
+  </si>
+  <si>
+    <t>chandan@test.com</t>
+  </si>
+  <si>
+    <t>test123</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -438,11 +442,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -468,14 +472,96 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{391F147B-AAA6-4678-8173-86354247A2D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="B2:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="ineuron@ineuron.ai" xr:uid="{51986416-36B7-4291-892B-BCAEC84834AF}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{31CE78CA-302C-4CB2-9172-19A498F89CF7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{4F5333F1-53DC-41B1-A508-B498EAC9087C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -486,8 +572,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -498,8 +584,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -510,32 +596,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
pushing correct working code
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{5D95B635-6528-4424-B668-2393BD27BC00}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{298EED56-8574-48B8-8117-10295A8EDAA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14415" windowHeight="6015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13725" windowHeight="6015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Sheet6" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J16"/>
+  <oleSize ref="A1:I16"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -528,7 +528,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>